<commit_message>
Constrained Euler implicit solving of axial fluxes in vessels
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25_07_02.xlsx
+++ b/simulations/scene/inputs/Scenarios_25_07_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp23939\home\torisuten\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\scene\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp46454\home\torisuten\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B82CE0-981E-4BAE-BBBC-CC80964E1D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC83FD6-F945-4EE9-B4CD-E7C8D1FCC29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="284">
   <si>
     <t>input_file</t>
   </si>
@@ -883,6 +883,9 @@
   </si>
   <si>
     <t>root02494.pckl</t>
+  </si>
+  <si>
+    <t>RC_ref_50 bck</t>
   </si>
 </sst>
 </file>
@@ -1812,13 +1815,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
+      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1834,7 @@
     <col min="8" max="20" width="39.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -1892,8 +1895,11 @@
       <c r="T1" s="13" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>208</v>
       </c>
@@ -1954,8 +1960,11 @@
       <c r="T2" s="7" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -2028,8 +2037,12 @@
         <f>4.18949994376799E-06/3600</f>
         <v>1.1637499843799972E-9</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="22">
+        <f>5.14350001490399E-06/3600</f>
+        <v>1.4287500041399972E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>185</v>
       </c>
@@ -2090,8 +2103,11 @@
       <c r="T4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
@@ -2152,8 +2168,11 @@
       <c r="T5" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X5" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>237</v>
       </c>
@@ -2227,8 +2246,12 @@
         <f t="shared" si="0"/>
         <v>4.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X6" s="10">
+        <f t="shared" ref="X6" si="1">0.00005 / 100</f>
+        <v>4.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
@@ -2289,8 +2312,11 @@
       <c r="T7" s="10">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X7" s="10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>243</v>
       </c>
@@ -2313,59 +2339,63 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="10">
-        <f t="shared" ref="H8:T8" si="1">0.00002 / 14</f>
+        <f t="shared" ref="H8:T8" si="2">0.00002 / 14</f>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="J8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="K8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="L8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="M8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="N8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="O8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="P8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="Q8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="R8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="S8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="T8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4285714285714286E-6</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X8" s="10">
+        <f t="shared" ref="X8" si="3">0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>194</v>
       </c>
@@ -2426,8 +2456,11 @@
       <c r="T9" s="10" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X9" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>195</v>
       </c>
@@ -2488,8 +2521,11 @@
       <c r="T10" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>196</v>
       </c>
@@ -2550,8 +2586,11 @@
       <c r="T11" s="10">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X11" s="10">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>202</v>
       </c>
@@ -2575,59 +2614,63 @@
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H12" s="20">
-        <f t="shared" ref="H12:T12" si="2">1250*0.000001/5</f>
+        <f t="shared" ref="H12:T12" si="4">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="J12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="T12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X12" s="20">
+        <f t="shared" ref="X12" si="5">1250*0.000001/5</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>205</v>
       </c>
@@ -2688,8 +2731,11 @@
       <c r="T13" s="15">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X13" s="15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>214</v>
       </c>
@@ -2712,59 +2758,63 @@
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="H14" s="10">
-        <f t="shared" ref="H14:T14" si="3" xml:space="preserve"> 0.0000000000025*10</f>
+        <f t="shared" ref="H14:T14" si="6" xml:space="preserve"> 0.0000000000025*10</f>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="L14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="M14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="Q14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="R14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="S14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-11</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X14" s="10">
+        <f t="shared" ref="X14" si="7" xml:space="preserve"> 0.0000000000025*10</f>
+        <v>2.4999999999999998E-11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>215</v>
       </c>
@@ -2787,59 +2837,63 @@
         <v>1.2E-8</v>
       </c>
       <c r="H15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" ref="H15:T15" si="8">0.00000000005 *2 / 100</f>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="I15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="J15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="K15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="L15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="M15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="N15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="O15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="P15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="Q15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="R15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
-      <c r="S15" s="10">
-        <f>0.00000000005 *2 / 100</f>
+      <c r="T15" s="10">
+        <f t="shared" si="8"/>
         <v>9.9999999999999998E-13</v>
       </c>
-      <c r="T15" s="10">
-        <f>0.00000000005 *2 / 100</f>
-        <v>9.9999999999999998E-13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X15" s="10">
+        <f>0.00000000005 *2/10</f>
+        <v>1.0000000000000001E-11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>247</v>
       </c>
@@ -2862,59 +2916,62 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" ref="H16:T16" si="9">0.0000001 * 10 /2 / 100 /2</f>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="I16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="J16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="K16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="L16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="M16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="N16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="O16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="P16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="Q16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="R16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="10">
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
-      <c r="S16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
+      <c r="T16" s="10">
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-9</v>
       </c>
-      <c r="T16" s="10">
-        <f>0.0000001 * 10 /2 / 100 /2</f>
-        <v>2.5000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X16" s="10">
+        <f>0.000000001</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>248</v>
       </c>
@@ -2975,8 +3032,11 @@
       <c r="T17" s="10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X17" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>216</v>
       </c>
@@ -2999,59 +3059,63 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" ref="H18:T18" si="4">0.000001 / 10000 / 4 / 10</f>
+        <f t="shared" ref="H18:T18" si="10">0.000001 / 10000 / 4 / 10</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="J18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="K18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="M18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="Q18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="R18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4999999999999998E-12</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X18" s="10">
+        <f t="shared" ref="X18" si="11">0.000001 / 10000 / 4 / 10</f>
+        <v>2.4999999999999998E-12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>217</v>
       </c>
@@ -3075,59 +3139,63 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" ref="H19:T19" si="5">0.00001</f>
+        <f t="shared" ref="H19:T19" si="12">0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="R19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X19" s="10">
+        <f t="shared" ref="X19" si="13">0.00001</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>250</v>
       </c>
@@ -3151,59 +3219,63 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" ref="H20:T20" si="6" xml:space="preserve"> 0.001 * 10</f>
+        <f t="shared" ref="H20:T20" si="14" xml:space="preserve"> 0.001 * 10</f>
         <v>0.01</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="Q20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="R20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X20" s="10">
+        <f t="shared" ref="X20" si="15" xml:space="preserve"> 0.001 * 10</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>252</v>
       </c>
@@ -3226,59 +3298,63 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" ref="H21:T21" si="7">0.00001 / 10 / 2 / 4</f>
+        <f t="shared" ref="H21:T21" si="16">0.00001 / 10 / 2 / 4</f>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="Q21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="R21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.2500000000000002E-7</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X21" s="10">
+        <f t="shared" ref="X21" si="17">0.00001 / 10 / 2 / 4</f>
+        <v>1.2500000000000002E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>218</v>
       </c>
@@ -3302,59 +3378,63 @@
         <v>0.10886399999999999</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" ref="H22:T22" si="8">0.84*(0.36^2)</f>
+        <f t="shared" ref="H22:T22" si="18">0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="Q22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="R22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.10886399999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X22" s="10">
+        <f t="shared" ref="X22" si="19">0.84*(0.36^2)</f>
+        <v>0.10886399999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>219</v>
       </c>
@@ -3415,8 +3495,11 @@
       <c r="T23" s="10">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X23" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>220</v>
       </c>
@@ -3477,8 +3560,11 @@
       <c r="T24" s="10" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X24" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>221</v>
       </c>
@@ -3502,59 +3588,63 @@
         <v>0.2</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" ref="H25:T25" si="9">2*0.1</f>
+        <f t="shared" ref="H25:T25" si="20">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="J25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="O25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="P25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="Q25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="R25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="S25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="T25" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X25" s="10">
+        <f t="shared" ref="X25" si="21">2*0.1</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>222</v>
       </c>
@@ -3615,8 +3705,11 @@
       <c r="T26" s="10">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X26" s="10">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>223</v>
       </c>
@@ -3639,59 +3732,63 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" ref="H27:T27" si="10">0.00001 /2</f>
+        <f t="shared" ref="H27:T27" si="22">0.00001 /2</f>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="M27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="O27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="P27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="Q27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="R27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="S27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="T27" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>5.0000000000000004E-6</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X27" s="10">
+        <f t="shared" ref="X27" si="23">0.00001 /2</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>254</v>
       </c>
@@ -3714,59 +3811,63 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" ref="H28:T28" si="11">0.000000005 / 5</f>
+        <f t="shared" ref="H28:T28" si="24">0.000000005 / 5</f>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="K28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="L28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="M28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="N28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="O28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="P28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="Q28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="R28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="S28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="T28" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X28" s="10">
+        <f t="shared" ref="X28" si="25">0.000000005 / 5</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>244</v>
       </c>
@@ -3786,7 +3887,7 @@
         <v>239</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29" si="12">0.00002 / 14 / 5</f>
+        <f t="shared" ref="G29" si="26">0.00002 / 14 / 5</f>
         <v>2.8571428571428575E-7</v>
       </c>
       <c r="H29" s="10">
@@ -3828,8 +3929,11 @@
       <c r="T29" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>245</v>
       </c>
@@ -3849,7 +3953,7 @@
         <v>239</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" ref="G30" si="13">0.00002 / 14 / 5 /10</f>
+        <f t="shared" ref="G30" si="27">0.00002 / 14 / 5 /10</f>
         <v>2.8571428571428575E-8</v>
       </c>
       <c r="H30" s="10">
@@ -3891,20 +3995,23 @@
       <c r="T30" s="10">
         <v>0</v>
       </c>
+      <c r="X30" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="colorScale" priority="524">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="525">
+    <cfRule type="colorScale" priority="561">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="560">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3916,17 +4023,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:T30">
-    <cfRule type="colorScale" priority="627">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="626">
+    <cfRule type="colorScale" priority="662">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="663">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H17">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3938,17 +4067,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:T6">
-    <cfRule type="colorScale" priority="630">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="629">
+    <cfRule type="colorScale" priority="666">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="665">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3960,17 +4089,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:T7">
-    <cfRule type="colorScale" priority="631">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="632">
+    <cfRule type="colorScale" priority="667">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="668">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3982,17 +4111,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:T8">
-    <cfRule type="colorScale" priority="634">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="633">
+    <cfRule type="colorScale" priority="670">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="669">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4004,17 +4133,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:T9">
-    <cfRule type="colorScale" priority="636">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="635">
+    <cfRule type="colorScale" priority="672">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="671">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4026,17 +4155,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:T10">
-    <cfRule type="colorScale" priority="638">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="637">
+    <cfRule type="colorScale" priority="674">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="673">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4048,17 +4177,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:T11">
-    <cfRule type="colorScale" priority="640">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="639">
+    <cfRule type="colorScale" priority="675">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="676">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4070,17 +4199,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:T14">
-    <cfRule type="colorScale" priority="642">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="641">
+    <cfRule type="colorScale" priority="678">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="677">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4092,17 +4221,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:T18">
-    <cfRule type="colorScale" priority="646">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="645">
+    <cfRule type="colorScale" priority="681">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="682">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4114,17 +4243,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:T20">
-    <cfRule type="colorScale" priority="664">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="665">
+    <cfRule type="colorScale" priority="701">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="700">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4136,17 +4265,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:T21">
-    <cfRule type="colorScale" priority="622">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="623">
+    <cfRule type="colorScale" priority="659">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="658">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4158,17 +4287,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:T22">
-    <cfRule type="colorScale" priority="648">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="647">
+    <cfRule type="colorScale" priority="683">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="684">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4180,17 +4309,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:T28">
-    <cfRule type="colorScale" priority="650">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="649">
+    <cfRule type="colorScale" priority="685">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="686">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4202,17 +4331,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:T30">
-    <cfRule type="colorScale" priority="624">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="625">
+    <cfRule type="colorScale" priority="661">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="660">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4224,17 +4353,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:I17">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4246,17 +4397,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J17">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4268,17 +4441,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:K17">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4290,17 +4485,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15:L17">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4312,17 +4529,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15:M17">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4334,17 +4573,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:N17">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4356,17 +4617,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15:O17">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4378,17 +4661,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15:P17">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4400,17 +4705,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15:Q17">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4422,17 +4749,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15 R17">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4444,17 +4793,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S15:S17 R16">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4466,281 +4837,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R15:R17">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:H17">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J17">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K17">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L15:L17">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M15:M17">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N17">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O17">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P15:P17">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q15:Q17">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S15:S17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4752,6 +4859,380 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15:T17">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X30">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X6">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X7">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X8">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X9">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X10">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X11">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X14">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X18">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X19:X20">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X21">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X22">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X23:X28">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X29:X30">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X15 X17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
debugged copy paste errors
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25_07_02.xlsx
+++ b/simulations/scene/inputs/Scenarios_25_07_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp46454\home\torisuten\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC83FD6-F945-4EE9-B4CD-E7C8D1FCC29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A089A219-9D47-4522-9F00-4DB938DDC3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1821,7 +1821,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
outputs for article figures
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25_07_02.xlsx
+++ b/simulations/scene/inputs/Scenarios_25_07_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp46454\home\torisuten\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A089A219-9D47-4522-9F00-4DB938DDC3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC730363-362B-4838-A83F-00B8BF67E4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="283">
   <si>
     <t>input_file</t>
   </si>
@@ -883,9 +883,6 @@
   </si>
   <si>
     <t>root02494.pckl</t>
-  </si>
-  <si>
-    <t>RC_ref_50 bck</t>
   </si>
 </sst>
 </file>
@@ -1815,13 +1812,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
+      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1831,7 @@
     <col min="8" max="20" width="39.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -1895,11 +1892,8 @@
       <c r="T1" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="X1" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>208</v>
       </c>
@@ -1960,11 +1954,8 @@
       <c r="T2" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -2037,12 +2028,8 @@
         <f>4.18949994376799E-06/3600</f>
         <v>1.1637499843799972E-9</v>
       </c>
-      <c r="X3" s="22">
-        <f>5.14350001490399E-06/3600</f>
-        <v>1.4287500041399972E-9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>185</v>
       </c>
@@ -2103,11 +2090,8 @@
       <c r="T4" s="7">
         <v>0</v>
       </c>
-      <c r="X4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
@@ -2168,11 +2152,8 @@
       <c r="T5" s="7">
         <v>20</v>
       </c>
-      <c r="X5" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>237</v>
       </c>
@@ -2246,12 +2227,8 @@
         <f t="shared" si="0"/>
         <v>4.9999999999999998E-7</v>
       </c>
-      <c r="X6" s="10">
-        <f t="shared" ref="X6" si="1">0.00005 / 100</f>
-        <v>4.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
@@ -2312,11 +2289,8 @@
       <c r="T7" s="10">
         <v>0.3</v>
       </c>
-      <c r="X7" s="10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>243</v>
       </c>
@@ -2339,63 +2313,59 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="10">
-        <f t="shared" ref="H8:T8" si="2">0.00002 / 14</f>
+        <f t="shared" ref="H8:T8" si="1">0.00002 / 14</f>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="J8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="K8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="L8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="M8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="N8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="O8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="P8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="Q8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="R8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="S8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
       <c r="T8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286E-6</v>
       </c>
-      <c r="X8" s="10">
-        <f t="shared" ref="X8" si="3">0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>194</v>
       </c>
@@ -2456,11 +2426,8 @@
       <c r="T9" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X9" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>195</v>
       </c>
@@ -2521,11 +2488,8 @@
       <c r="T10" s="10">
         <v>0</v>
       </c>
-      <c r="X10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>196</v>
       </c>
@@ -2586,11 +2550,8 @@
       <c r="T11" s="10">
         <v>1E-3</v>
       </c>
-      <c r="X11" s="10">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>202</v>
       </c>
@@ -2614,63 +2575,59 @@
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H12" s="20">
-        <f t="shared" ref="H12:T12" si="4">1250*0.000001/5</f>
+        <f t="shared" ref="H12:T12" si="2">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="J12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="T12" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="X12" s="20">
-        <f t="shared" ref="X12" si="5">1250*0.000001/5</f>
-        <v>2.5000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>205</v>
       </c>
@@ -2731,11 +2688,8 @@
       <c r="T13" s="15">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="X13" s="15">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>214</v>
       </c>
@@ -2758,63 +2712,59 @@
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="H14" s="10">
-        <f t="shared" ref="H14:T14" si="6" xml:space="preserve"> 0.0000000000025*10</f>
+        <f t="shared" ref="H14:T14" si="3" xml:space="preserve"> 0.0000000000025*10</f>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="L14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="M14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="Q14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="R14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="S14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2.4999999999999998E-11</v>
       </c>
-      <c r="X14" s="10">
-        <f t="shared" ref="X14" si="7" xml:space="preserve"> 0.0000000000025*10</f>
-        <v>2.4999999999999998E-11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>215</v>
       </c>
@@ -2837,63 +2787,59 @@
         <v>1.2E-8</v>
       </c>
       <c r="H15" s="10">
-        <f t="shared" ref="H15:T15" si="8">0.00000000005 *2 / 100</f>
+        <f t="shared" ref="H15" si="4">0.00000000005 *2 / 100</f>
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="J15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="K15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="L15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="M15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="Q15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="R15" s="10">
         <f>0.00000000005 *2</f>
         <v>1E-10</v>
       </c>
       <c r="S15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
       </c>
       <c r="T15" s="10">
-        <f t="shared" si="8"/>
-        <v>9.9999999999999998E-13</v>
-      </c>
-      <c r="X15" s="10">
-        <f>0.00000000005 *2/10</f>
-        <v>1.0000000000000001E-11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+        <f>0.00000000005 *2</f>
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>247</v>
       </c>
@@ -2916,62 +2862,47 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H16" s="10">
-        <f t="shared" ref="H16:T16" si="9">0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" ref="H16" si="5">0.0000001 * 10 /2 / 100 /2</f>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="M16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="R16" s="10">
         <v>0</v>
       </c>
       <c r="S16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
+        <v>0</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-9</v>
-      </c>
-      <c r="X16" s="10">
-        <f>0.000000001</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>248</v>
       </c>
@@ -3032,11 +2963,8 @@
       <c r="T17" s="10">
         <v>1000</v>
       </c>
-      <c r="X17" s="10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>216</v>
       </c>
@@ -3059,63 +2987,59 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" ref="H18:T18" si="10">0.000001 / 10000 / 4 / 10</f>
+        <f t="shared" ref="H18:T18" si="6">0.000001 / 10000 / 4 / 10</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="J18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="K18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="M18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="Q18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="R18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.4999999999999998E-12</v>
       </c>
-      <c r="X18" s="10">
-        <f t="shared" ref="X18" si="11">0.000001 / 10000 / 4 / 10</f>
-        <v>2.4999999999999998E-12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>217</v>
       </c>
@@ -3139,63 +3063,59 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" ref="H19:T19" si="12">0.00001</f>
+        <f t="shared" ref="H19:T19" si="7">0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="R19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="X19" s="10">
-        <f t="shared" ref="X19" si="13">0.00001</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>250</v>
       </c>
@@ -3219,63 +3139,59 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" ref="H20:T20" si="14" xml:space="preserve"> 0.001 * 10</f>
+        <f t="shared" ref="H20:T20" si="8" xml:space="preserve"> 0.001 * 10</f>
         <v>0.01</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="Q20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="R20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
-      <c r="X20" s="10">
-        <f t="shared" ref="X20" si="15" xml:space="preserve"> 0.001 * 10</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>252</v>
       </c>
@@ -3298,63 +3214,59 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" ref="H21:T21" si="16">0.00001 / 10 / 2 / 4</f>
+        <f t="shared" ref="H21:T21" si="9">0.00001 / 10 / 2 / 4</f>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="Q21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="R21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000002E-7</v>
       </c>
-      <c r="X21" s="10">
-        <f t="shared" ref="X21" si="17">0.00001 / 10 / 2 / 4</f>
-        <v>1.2500000000000002E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>218</v>
       </c>
@@ -3378,63 +3290,59 @@
         <v>0.10886399999999999</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" ref="H22:T22" si="18">0.84*(0.36^2)</f>
+        <f t="shared" ref="H22:T22" si="10">0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="Q22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="R22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>0.10886399999999999</v>
       </c>
-      <c r="X22" s="10">
-        <f t="shared" ref="X22" si="19">0.84*(0.36^2)</f>
-        <v>0.10886399999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>219</v>
       </c>
@@ -3495,11 +3403,8 @@
       <c r="T23" s="10">
         <v>0.2</v>
       </c>
-      <c r="X23" s="10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>220</v>
       </c>
@@ -3560,11 +3465,8 @@
       <c r="T24" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X24" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>221</v>
       </c>
@@ -3588,63 +3490,59 @@
         <v>0.2</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" ref="H25:T25" si="20">2*0.1</f>
+        <f t="shared" ref="H25:T25" si="11">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="J25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="O25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="P25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="Q25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="R25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="S25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="T25" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
-      <c r="X25" s="10">
-        <f t="shared" ref="X25" si="21">2*0.1</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>222</v>
       </c>
@@ -3705,11 +3603,8 @@
       <c r="T26" s="10">
         <v>1E-3</v>
       </c>
-      <c r="X26" s="10">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>223</v>
       </c>
@@ -3732,63 +3627,59 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" ref="H27:T27" si="22">0.00001 /2</f>
+        <f t="shared" ref="H27:T27" si="12">0.00001 /2</f>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="M27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="O27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="P27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="Q27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="R27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="S27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="T27" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="X27" s="10">
-        <f t="shared" ref="X27" si="23">0.00001 /2</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>254</v>
       </c>
@@ -3811,63 +3702,59 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" ref="H28:T28" si="24">0.000000005 / 5</f>
+        <f t="shared" ref="H28:T28" si="13">0.000000005 / 5</f>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="K28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="L28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="M28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="N28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="O28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="P28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="Q28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="R28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="S28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="T28" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="X28" s="10">
-        <f t="shared" ref="X28" si="25">0.000000005 / 5</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>244</v>
       </c>
@@ -3887,7 +3774,7 @@
         <v>239</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29" si="26">0.00002 / 14 / 5</f>
+        <f t="shared" ref="G29" si="14">0.00002 / 14 / 5</f>
         <v>2.8571428571428575E-7</v>
       </c>
       <c r="H29" s="10">
@@ -3929,11 +3816,8 @@
       <c r="T29" s="10">
         <v>0</v>
       </c>
-      <c r="X29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>245</v>
       </c>
@@ -3953,7 +3837,7 @@
         <v>239</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" ref="G30" si="27">0.00002 / 14 / 5 /10</f>
+        <f t="shared" ref="G30" si="15">0.00002 / 14 / 5 /10</f>
         <v>2.8571428571428575E-8</v>
       </c>
       <c r="H30" s="10">
@@ -3995,23 +3879,20 @@
       <c r="T30" s="10">
         <v>0</v>
       </c>
-      <c r="X30" s="10">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="colorScale" priority="561">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="560">
+    <cfRule type="colorScale" priority="592">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="593">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4023,17 +3904,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:T30">
-    <cfRule type="colorScale" priority="662">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="663">
+    <cfRule type="colorScale" priority="694">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="695">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4045,17 +3926,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H17">
-    <cfRule type="colorScale" priority="59">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="60">
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4067,17 +3948,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:T6">
-    <cfRule type="colorScale" priority="666">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="665">
+    <cfRule type="colorScale" priority="697">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="698">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4089,17 +3970,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:T7">
-    <cfRule type="colorScale" priority="667">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="668">
+    <cfRule type="colorScale" priority="699">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="700">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4111,17 +3992,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:T8">
-    <cfRule type="colorScale" priority="670">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="669">
+    <cfRule type="colorScale" priority="701">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="702">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4133,17 +4014,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:T9">
-    <cfRule type="colorScale" priority="672">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="671">
+    <cfRule type="colorScale" priority="703">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="704">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4155,17 +4036,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:T10">
-    <cfRule type="colorScale" priority="674">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="673">
+    <cfRule type="colorScale" priority="705">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="706">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4177,17 +4058,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:T11">
-    <cfRule type="colorScale" priority="675">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="676">
+    <cfRule type="colorScale" priority="707">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="708">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4199,17 +4080,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:T14">
-    <cfRule type="colorScale" priority="678">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="677">
+    <cfRule type="colorScale" priority="709">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="710">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4221,17 +4102,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:T18">
-    <cfRule type="colorScale" priority="681">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="682">
+    <cfRule type="colorScale" priority="713">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="714">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4243,17 +4124,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:T20">
-    <cfRule type="colorScale" priority="701">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="700">
+    <cfRule type="colorScale" priority="732">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="733">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4265,17 +4146,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:T21">
-    <cfRule type="colorScale" priority="659">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="658">
+    <cfRule type="colorScale" priority="690">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="691">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4287,17 +4168,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:T22">
-    <cfRule type="colorScale" priority="683">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="684">
+    <cfRule type="colorScale" priority="715">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="716">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4309,17 +4190,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:T28">
-    <cfRule type="colorScale" priority="685">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="686">
+    <cfRule type="colorScale" priority="717">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="718">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4331,17 +4212,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:T30">
-    <cfRule type="colorScale" priority="661">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="660">
+    <cfRule type="colorScale" priority="692">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="693">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4353,39 +4234,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="88">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I17">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="58">
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4397,39 +4256,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="85">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J17">
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4441,39 +4278,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="colorScale" priority="84">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K17">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4485,39 +4300,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="colorScale" priority="82">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="81">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L15:L17">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4529,39 +4322,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="colorScale" priority="79">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="80">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M15:M17">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4573,39 +4344,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="colorScale" priority="78">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="77">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N17">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="109">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4617,39 +4366,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="colorScale" priority="76">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="75">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O17">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4661,39 +4388,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="colorScale" priority="74">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="73">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P15:P17">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="105">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4705,39 +4410,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="colorScale" priority="72">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="71">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q15:Q17">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4749,17 +4432,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="colorScale" priority="69">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4770,18 +4453,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R15 R17">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="61">
+  <conditionalFormatting sqref="Q15:T15 Q17:T17">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4793,17 +4476,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4814,18 +4497,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S15:S17 R16">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="Q16:T16">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4837,17 +4520,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="95">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4858,18 +4541,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T15:T17">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="I15 I17">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4880,7 +4563,205 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X30">
+  <conditionalFormatting sqref="I16">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15 J17">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15 K17">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15 L17">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15 M17">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M16">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15 N17">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4902,18 +4783,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X6">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4924,18 +4805,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X7">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="O15 O17">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4946,18 +4827,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X8">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="O16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4968,18 +4849,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X9">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="P15 P17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4990,249 +4871,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X10">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X11">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X14">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X18">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X19:X20">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X21">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X22">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X23:X28">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X29:X30">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X15 X17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X16">
+  <conditionalFormatting sqref="P16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
intermediate commit correcting advection
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25_07_02.xlsx
+++ b/simulations/scene/inputs/Scenarios_25_07_02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp46454\home\torisuten\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\scene\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp54592\home\torisuten\package\Root-CyNAPS\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC730363-362B-4838-A83F-00B8BF67E4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD89404-3AF7-4DB7-8570-8570461BF443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1818,7 +1818,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
+      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,51 +2791,51 @@
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="I15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" ref="I15:T15" si="5">0.00000000005 *2</f>
         <v>1E-10</v>
       </c>
       <c r="J15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="K15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="L15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="M15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="N15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="O15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="P15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="Q15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="R15" s="10">
-        <f>0.00000000005 *2</f>
+        <f>0.00000000005 *2 * 2</f>
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
-      <c r="S15" s="10">
-        <f>0.00000000005 *2</f>
-        <v>1E-10</v>
-      </c>
       <c r="T15" s="10">
-        <f>0.00000000005 *2</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
     </row>
@@ -2862,7 +2862,7 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H16" s="10">
-        <f t="shared" ref="H16" si="5">0.0000001 * 10 /2 / 100 /2</f>
+        <f t="shared" ref="H16" si="6">0.0000001 * 10 /2 / 100 /2</f>
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="I16" s="10">
@@ -2987,55 +2987,55 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" ref="H18:T18" si="6">0.000001 / 10000 / 4 / 10</f>
+        <f t="shared" ref="H18:T18" si="7">0.000001 / 10000 / 4 / 10</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="J18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="K18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="M18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="Q18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="R18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4999999999999998E-12</v>
       </c>
     </row>
@@ -3063,55 +3063,55 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" ref="H19:T19" si="7">0.00001</f>
+        <f t="shared" ref="H19:T19" si="8">0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="R19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
@@ -3139,55 +3139,55 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" ref="H20:T20" si="8" xml:space="preserve"> 0.001 * 10</f>
+        <f t="shared" ref="H20:T20" si="9" xml:space="preserve"> 0.001 * 10</f>
         <v>0.01</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="Q20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="R20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
     </row>
@@ -3214,55 +3214,55 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" ref="H21:T21" si="9">0.00001 / 10 / 2 / 4</f>
+        <f t="shared" ref="H21:T21" si="10">0.00001 / 10 / 2 / 4</f>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="Q21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="R21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2500000000000002E-7</v>
       </c>
     </row>
@@ -3290,55 +3290,55 @@
         <v>0.10886399999999999</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" ref="H22:T22" si="10">0.84*(0.36^2)</f>
+        <f t="shared" ref="H22:T22" si="11">0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="Q22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="R22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10886399999999999</v>
       </c>
     </row>
@@ -3490,55 +3490,55 @@
         <v>0.2</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" ref="H25:T25" si="11">2*0.1</f>
+        <f t="shared" ref="H25:T25" si="12">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="J25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="O25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="P25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="Q25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="R25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="S25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="T25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3627,55 +3627,55 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" ref="H27:T27" si="12">0.00001 /2</f>
+        <f t="shared" ref="H27:T27" si="13">0.00001 /2</f>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="M27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="O27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="P27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="Q27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="R27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="S27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="T27" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
@@ -3702,55 +3702,55 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" ref="H28:T28" si="13">0.000000005 / 5</f>
+        <f t="shared" ref="H28:T28" si="14">0.000000005 / 5</f>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="K28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="L28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="M28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="N28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="O28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="P28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="Q28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="R28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="S28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="T28" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
@@ -3774,7 +3774,7 @@
         <v>239</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29" si="14">0.00002 / 14 / 5</f>
+        <f t="shared" ref="G29" si="15">0.00002 / 14 / 5</f>
         <v>2.8571428571428575E-7</v>
       </c>
       <c r="H29" s="10">
@@ -3837,7 +3837,7 @@
         <v>239</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" ref="G30" si="15">0.00002 / 14 / 5 /10</f>
+        <f t="shared" ref="G30" si="16">0.00002 / 14 / 5 /10</f>
         <v>2.8571428571428575E-8</v>
       </c>
       <c r="H30" s="10">
@@ -3882,17 +3882,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G29:G30">
+    <cfRule type="colorScale" priority="593">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="592">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="593">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3926,17 +3926,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H17">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="91">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3970,17 +3970,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:T7">
+    <cfRule type="colorScale" priority="700">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="699">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="700">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3992,17 +3992,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:T8">
+    <cfRule type="colorScale" priority="702">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="701">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="702">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4036,17 +4036,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:T10">
+    <cfRule type="colorScale" priority="706">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="705">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="706">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4080,17 +4080,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:T14">
+    <cfRule type="colorScale" priority="710">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="709">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="710">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4102,17 +4102,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:T18">
+    <cfRule type="colorScale" priority="714">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="713">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="714">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4124,17 +4124,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:T20">
+    <cfRule type="colorScale" priority="733">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="732">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="733">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4146,17 +4146,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:T21">
+    <cfRule type="colorScale" priority="691">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="690">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="691">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4190,17 +4190,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:T28">
+    <cfRule type="colorScale" priority="718">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="717">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="718">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4212,17 +4212,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:T30">
+    <cfRule type="colorScale" priority="693">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="692">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="693">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4234,6 +4234,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
@@ -4244,7 +4254,41 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="120">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15 I17">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4277,7 +4321,61 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J15 J17">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K3">
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
@@ -4288,7 +4386,41 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="116">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15 K17">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4321,6 +4453,50 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L15 L17">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M3">
     <cfRule type="colorScale" priority="111">
       <colorScale>
@@ -4333,6 +4509,50 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15 M17">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M16">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4365,6 +4585,50 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N15 N17">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O3">
     <cfRule type="colorScale" priority="107">
       <colorScale>
@@ -4377,6 +4641,50 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15 O17">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4409,6 +4717,50 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P15 P17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
     <cfRule type="colorScale" priority="103">
       <colorScale>
@@ -4421,6 +4773,50 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="104">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15:T15 Q17:T17">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="94">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16:T16">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4453,28 +4849,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q15:T15 Q17:T17">
-    <cfRule type="colorScale" priority="93">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="94">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S3">
     <cfRule type="colorScale" priority="99">
       <colorScale>
@@ -4497,392 +4871,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q16:T16">
-    <cfRule type="colorScale" priority="71">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="72">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="T3">
+    <cfRule type="colorScale" priority="96">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="95">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="96">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15 I17">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15 J17">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15 K17">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L15 L17">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M15 M17">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15 N17">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O15 O17">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P15 P17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P16">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>